<commit_message>
Make headless for MainRun_PK with updated stage transitions and a vaccination speed of 0%.
</commit_message>
<xml_diff>
--- a/Pakistan/input/stageParams.xlsx
+++ b/Pakistan/input/stageParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\CovidABM\Pakistan\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12CB615-C414-4312-BF3E-5BE46AE5D364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7B84D7-C494-4DC2-8A89-68FD72A967B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA71E6BA-EB7A-46FB-96A7-55CE21DF9A5D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA71E6BA-EB7A-46FB-96A7-55CE21DF9A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Stage 1</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Chance of someone teleporting to a random visit location anywhere in the country.</t>
+  </si>
+  <si>
+    <t>Enter when 7 day cases &gt;</t>
+  </si>
+  <si>
+    <t>Leave when 7 day cases &lt;</t>
+  </si>
+  <si>
+    <t>For moderate supress and moderate_suppress_no_4, the only policy in the model</t>
   </si>
 </sst>
 </file>
@@ -457,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E08A201-B651-460B-93FA-4A9CD9E4EB28}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,6 +692,46 @@
         <v>23</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>5600</v>
+      </c>
+      <c r="D12">
+        <v>11200</v>
+      </c>
+      <c r="E12">
+        <v>22400</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>3733</v>
+      </c>
+      <c r="D13">
+        <v>7466</v>
+      </c>
+      <c r="E13">
+        <v>14933</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix stage 2 skipping.
</commit_message>
<xml_diff>
--- a/Pakistan/input/stageParams.xlsx
+++ b/Pakistan/input/stageParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\CovidABM\Pakistan\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7B84D7-C494-4DC2-8A89-68FD72A967B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BA139F-D74E-4757-BBFA-480352433C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA71E6BA-EB7A-46FB-96A7-55CE21DF9A5D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA71E6BA-EB7A-46FB-96A7-55CE21DF9A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Stage 1</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>For moderate supress and moderate_suppress_no_4, the only policy in the model</t>
+  </si>
+  <si>
+    <t>Approx. Calibrate R0</t>
+  </si>
+  <si>
+    <t>Stage 2b</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -138,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,12 +155,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,270 +491,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E08A201-B651-460B-93FA-4A9CD9E4EB28}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="13.7109375" customWidth="1"/>
+    <col min="2" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="E2" s="1">
         <v>3.3</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>45</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>70</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1">
         <v>78</v>
       </c>
-      <c r="E3">
+      <c r="F3" s="1">
         <v>93</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>45</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>70</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1">
         <v>78</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="1">
         <v>93</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>35</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>54</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1">
         <v>62</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="1">
         <v>86</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>75</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>54</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1">
         <v>25</v>
       </c>
-      <c r="E6">
+      <c r="F6" s="1">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="b">
+      <c r="B7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C7" t="b">
+      <c r="C7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D7" t="b">
+      <c r="D7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E7" t="b">
+      <c r="F7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>35</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>50</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1">
         <v>75</v>
       </c>
-      <c r="E8">
+      <c r="F8" s="1">
         <v>90</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
         <v>5</v>
       </c>
-      <c r="E9">
+      <c r="F9" s="1">
         <v>2.5</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="E10" s="1">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="1">
         <v>0.03</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="E11" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="E11">
+      <c r="F11" s="1">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>5600</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1">
         <v>11200</v>
       </c>
-      <c r="E12">
+      <c r="F12" s="1">
         <v>22400</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>3733</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1">
         <v>7466</v>
       </c>
-      <c r="E13">
+      <c r="F13" s="1">
         <v>14933</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.82</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP stage parameter tweaking.
</commit_message>
<xml_diff>
--- a/Pakistan/input/stageParams.xlsx
+++ b/Pakistan/input/stageParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\CovidABM\Pakistan\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BA139F-D74E-4757-BBFA-480352433C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EACD362-22B8-4975-8BF5-0E207767600F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA71E6BA-EB7A-46FB-96A7-55CE21DF9A5D}"/>
+    <workbookView xWindow="30975" yWindow="945" windowWidth="25035" windowHeight="13980" xr2:uid="{DA71E6BA-EB7A-46FB-96A7-55CE21DF9A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Stage 1</t>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Stage 0</t>
+  </si>
+  <si>
+    <t>traceMult</t>
+  </si>
+  <si>
+    <t>case_isolation</t>
+  </si>
+  <si>
+    <t>Whether tracked cases isolate and cause their household to isolate.</t>
+  </si>
+  <si>
+    <t>Multiplier for the proportion of people tracked each day, which itself varies based on case load.</t>
   </si>
 </sst>
 </file>
@@ -491,152 +506,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E08A201-B651-460B-93FA-4A9CD9E4EB28}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="94.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>6.5</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>3.3</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
         <v>45</v>
-      </c>
-      <c r="C3" s="1">
-        <v>70</v>
       </c>
       <c r="D3" s="1">
         <v>70</v>
       </c>
       <c r="E3" s="1">
+        <v>70</v>
+      </c>
+      <c r="F3" s="1">
         <v>78</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>93</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <v>45</v>
-      </c>
-      <c r="C4" s="1">
-        <v>70</v>
       </c>
       <c r="D4" s="1">
         <v>70</v>
       </c>
       <c r="E4" s="1">
+        <v>70</v>
+      </c>
+      <c r="F4" s="1">
         <v>78</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>93</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
         <v>35</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>54</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>60</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>62</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>86</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1">
         <v>75</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>54</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>45</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>25</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -650,172 +686,249 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
         <v>35</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>50</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>55</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>75</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>90</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1">
         <v>9</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>7</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>6</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>5</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>2.5</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.14280000000000001</v>
       </c>
       <c r="C10" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="D10" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E10" s="1">
         <v>0.13</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>0.03</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>7.4999999999999997E-3</v>
+        <v>0.05</v>
       </c>
       <c r="C11" s="1">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="D11" s="1">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="E11" s="1">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
         <v>5600</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F14" s="1">
         <v>11200</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G14" s="1">
         <v>22400</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
         <v>3733</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F15" s="1">
         <v>7466</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G15" s="1">
         <v>14933</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="1">
         <v>1.82</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D16" s="1">
         <v>1.35</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E16" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F16" s="1">
         <v>0.89</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G16" s="1">
         <v>0.77</v>
       </c>
+      <c r="H16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweak stages for Tony.
</commit_message>
<xml_diff>
--- a/Pakistan/input/stageParams.xlsx
+++ b/Pakistan/input/stageParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\CovidABM\Pakistan\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EACD362-22B8-4975-8BF5-0E207767600F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548B37C1-2C02-4AEF-B971-81A32922EF60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30975" yWindow="945" windowWidth="25035" windowHeight="13980" xr2:uid="{DA71E6BA-EB7A-46FB-96A7-55CE21DF9A5D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA71E6BA-EB7A-46FB-96A7-55CE21DF9A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,16 +550,16 @@
         <v>20</v>
       </c>
       <c r="C2" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="E2" s="1">
         <v>6.5</v>
       </c>
       <c r="F2" s="1">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -585,10 +585,10 @@
         <v>70</v>
       </c>
       <c r="F3" s="1">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G3" s="1">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
@@ -611,10 +611,10 @@
         <v>70</v>
       </c>
       <c r="F4" s="1">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G4" s="1">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>16</v>
@@ -631,16 +631,16 @@
         <v>35</v>
       </c>
       <c r="D5" s="1">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1">
         <v>60</v>
       </c>
       <c r="F5" s="1">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G5" s="1">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
@@ -657,7 +657,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="1">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1">
         <v>45</v>
@@ -718,7 +718,7 @@
         <v>75</v>
       </c>
       <c r="G8" s="1">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>21</v>
@@ -744,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>20</v>
@@ -758,10 +758,10 @@
         <v>0.14280000000000001</v>
       </c>
       <c r="C10" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>0.14000000000000001</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="E10" s="1">
         <v>0.13</v>
@@ -796,7 +796,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="G11" s="1">
-        <v>2.5000000000000001E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>23</v>
@@ -914,19 +914,19 @@
         <v>2.5</v>
       </c>
       <c r="C16" s="1">
-        <v>1.82</v>
+        <v>1.8</v>
       </c>
       <c r="D16" s="1">
-        <v>1.35</v>
+        <v>1.22</v>
       </c>
       <c r="E16" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="F16" s="1">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="G16" s="1">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="H16" s="1"/>
     </row>

</xml_diff>